<commit_message>
Documentos de pruebas individuales Stacy
</commit_message>
<xml_diff>
--- a/Sprint#5/pruebas individuales Stacy/Log pruebas individuales RF-23.xlsx
+++ b/Sprint#5/pruebas individuales Stacy/Log pruebas individuales RF-23.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Oscar\Documents\GitHub\SIGAB\SIGAB\Sprint#5\pruebas individuales Oscar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\STACY\Documents\GitHub\SIGAB\Sprint#5\pruebas individuales Stacy\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27CF554-9C3E-4696-831B-694406E1E453}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RF 20" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Observación</t>
   </si>
@@ -78,37 +79,29 @@
     <t>X</t>
   </si>
   <si>
-    <t>Plan gesti[on de redes sociales Ebdi (PDF)</t>
-  </si>
-  <si>
-    <t>Ejemplo asistencia Conferencia (PDF)</t>
-  </si>
-  <si>
-    <t>Cuadro Informe Redes Sociales (PDF)</t>
-  </si>
-  <si>
-    <t>Imágen de evidencia de actividad realizada por la EBDI (Imágen)</t>
-  </si>
-  <si>
-    <t>Taller Portafolio Bibliotecas (PDF)</t>
-  </si>
-  <si>
-    <t>Datos pruebas actividades (EXCEL)</t>
-  </si>
-  <si>
-    <t>Oscar Alvarado Gutiérrez</t>
-  </si>
-  <si>
     <t>Autorizar una actividad interna.</t>
   </si>
   <si>
     <t>La verificación es brindada únicamente por un usuario autorizado de la administración</t>
+  </si>
+  <si>
+    <t>Stacy Gonzalez Santamaria</t>
+  </si>
+  <si>
+    <t>Actividad Interna:  Tema: Estudio de la realidad nacional, Responsable de coordinar actividad: 
+Kattia Bermúdez León, Estado: Ejecutada, Proposito:Otro, Tipo de actividad: Co-Curricular, Fecha: 05/20/2019</t>
+  </si>
+  <si>
+    <t>Personal:  Jenny Ulate Montero</t>
+  </si>
+  <si>
+    <t>El personal acorde al privilegio de su rol, logra autorizar correctamente la actividad antes de ser desplegada a otros usuarios.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -179,14 +172,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,8 +186,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,33 +226,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -278,17 +251,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -317,7 +286,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -330,39 +314,19 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Cálculo" xfId="2" builtinId="22"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -382,60 +346,43 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>426721</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>120361</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A708F16F-7A7C-43B3-96D9-7956B2A00F35}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A7A9FE3-CFFD-4C70-8125-F2B9E17E86A3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="11715750" cy="8648700"/>
+          <a:off x="1" y="0"/>
+          <a:ext cx="8351520" cy="4143721"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -463,7 +410,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{77B5A9F6-0714-411B-A079-BBA359F1F23B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77B5A9F6-0714-411B-A079-BBA359F1F23B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -805,228 +752,177 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="64.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="64.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
     <col min="5" max="5" width="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" ht="98.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="98.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>18</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-    </row>
-    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+    </row>
+    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="11">
-        <v>30</v>
-      </c>
-      <c r="C5" s="21" t="s">
+      <c r="B5" s="10">
         <v>23</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="C5" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="B6" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>44334</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="14" t="s">
+    <row r="11" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="C11" s="5"/>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="31"/>
-    </row>
-    <row r="13" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-    </row>
-    <row r="17" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+    </row>
+    <row r="13" spans="1:6" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="26"/>
-    </row>
-    <row r="18" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1043,12 +939,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1056,12 +952,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>